<commit_message>
SE 2018 test1 score commit
</commit_message>
<xml_diff>
--- a/Grade 2018/Class Test/CT_Summary_YC_2018.xlsx
+++ b/Grade 2018/Class Test/CT_Summary_YC_2018.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\NIIT\NIIT教案\Sept-2020---Jan-2021\Grade 2018\Class Test\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6B8BC82D-790D-4151-A283-92204FE10705}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4D876AFA-BC2C-4BEB-8A8D-808B7AD34324}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="CS1" sheetId="2" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="635" uniqueCount="381">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="634" uniqueCount="381">
   <si>
     <t>No</t>
   </si>
@@ -4285,8 +4285,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{95DDB66F-D270-42E2-B6F1-6326C25DE7DB}">
   <dimension ref="A1:J51"/>
   <sheetViews>
-    <sheetView zoomScale="50" zoomScaleNormal="50" workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+    <sheetView tabSelected="1" topLeftCell="A34" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="F50" sqref="F50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -4356,8 +4356,8 @@
       <c r="C3" s="11"/>
       <c r="D3" s="14"/>
       <c r="E3" s="17"/>
-      <c r="F3" s="3" t="s">
-        <v>12</v>
+      <c r="F3" s="3">
+        <v>44096</v>
       </c>
       <c r="G3" s="3" t="s">
         <v>12</v>
@@ -4386,13 +4386,15 @@
       <c r="E4" s="9" t="e">
         <v>#N/A</v>
       </c>
-      <c r="F4" s="7"/>
+      <c r="F4" s="7">
+        <v>0</v>
+      </c>
       <c r="G4" s="7"/>
       <c r="H4" s="7"/>
       <c r="I4" s="7"/>
-      <c r="J4" s="6" t="e">
+      <c r="J4" s="6">
         <f>AVERAGE(F4:I4)</f>
-        <v>#DIV/0!</v>
+        <v>0</v>
       </c>
     </row>
     <row r="5" spans="1:10" ht="16.5" x14ac:dyDescent="0.15">
@@ -4411,13 +4413,15 @@
       <c r="E5" s="9" t="s">
         <v>161</v>
       </c>
-      <c r="F5" s="7"/>
+      <c r="F5" s="7">
+        <v>8</v>
+      </c>
       <c r="G5" s="7"/>
       <c r="H5" s="7"/>
       <c r="I5" s="7"/>
-      <c r="J5" s="6" t="e">
+      <c r="J5" s="6">
         <f>AVERAGE(F5:I5)</f>
-        <v>#DIV/0!</v>
+        <v>8</v>
       </c>
     </row>
     <row r="6" spans="1:10" ht="16.5" x14ac:dyDescent="0.15">
@@ -4436,13 +4440,15 @@
       <c r="E6" s="9" t="s">
         <v>86</v>
       </c>
-      <c r="F6" s="7"/>
+      <c r="F6" s="7">
+        <v>8</v>
+      </c>
       <c r="G6" s="7"/>
       <c r="H6" s="7"/>
       <c r="I6" s="7"/>
-      <c r="J6" s="6" t="e">
+      <c r="J6" s="6">
         <f>AVERAGE(F6:I6)</f>
-        <v>#DIV/0!</v>
+        <v>8</v>
       </c>
     </row>
     <row r="7" spans="1:10" ht="16.5" x14ac:dyDescent="0.15">
@@ -4461,13 +4467,15 @@
       <c r="E7" s="9" t="s">
         <v>236</v>
       </c>
-      <c r="F7" s="7"/>
+      <c r="F7" s="7">
+        <v>10</v>
+      </c>
       <c r="G7" s="7"/>
       <c r="H7" s="7"/>
       <c r="I7" s="7"/>
-      <c r="J7" s="6" t="e">
+      <c r="J7" s="6">
         <f>AVERAGE(F7:I7)</f>
-        <v>#DIV/0!</v>
+        <v>10</v>
       </c>
     </row>
     <row r="8" spans="1:10" ht="16.5" x14ac:dyDescent="0.15">
@@ -4486,13 +4494,15 @@
       <c r="E8" s="9" t="s">
         <v>364</v>
       </c>
-      <c r="F8" s="7"/>
+      <c r="F8" s="7">
+        <v>10</v>
+      </c>
       <c r="G8" s="7"/>
       <c r="H8" s="7"/>
       <c r="I8" s="7"/>
-      <c r="J8" s="6" t="e">
+      <c r="J8" s="6">
         <f>AVERAGE(F8,G8)</f>
-        <v>#DIV/0!</v>
+        <v>10</v>
       </c>
     </row>
     <row r="9" spans="1:10" ht="16.5" x14ac:dyDescent="0.15">
@@ -4511,13 +4521,15 @@
       <c r="E9" s="9" t="s">
         <v>162</v>
       </c>
-      <c r="F9" s="7"/>
+      <c r="F9" s="7">
+        <v>10</v>
+      </c>
       <c r="G9" s="7"/>
       <c r="H9" s="7"/>
       <c r="I9" s="7"/>
-      <c r="J9" s="6" t="e">
+      <c r="J9" s="6">
         <f>AVERAGE(F9:I9)</f>
-        <v>#DIV/0!</v>
+        <v>10</v>
       </c>
     </row>
     <row r="10" spans="1:10" ht="16.5" x14ac:dyDescent="0.15">
@@ -4536,13 +4548,15 @@
       <c r="E10" s="9" t="s">
         <v>314</v>
       </c>
-      <c r="F10" s="7"/>
+      <c r="F10" s="7">
+        <v>9</v>
+      </c>
       <c r="G10" s="7"/>
       <c r="H10" s="7"/>
       <c r="I10" s="7"/>
-      <c r="J10" s="6" t="e">
+      <c r="J10" s="6">
         <f>AVERAGE(F10:I10)</f>
-        <v>#DIV/0!</v>
+        <v>9</v>
       </c>
     </row>
     <row r="11" spans="1:10" ht="16.5" x14ac:dyDescent="0.15">
@@ -4561,13 +4575,15 @@
       <c r="E11" s="9" t="s">
         <v>8</v>
       </c>
-      <c r="F11" s="7"/>
+      <c r="F11" s="7">
+        <v>9</v>
+      </c>
       <c r="G11" s="7"/>
       <c r="H11" s="7"/>
       <c r="I11" s="7"/>
-      <c r="J11" s="6" t="e">
+      <c r="J11" s="6">
         <f>AVERAGE(F11:I11)</f>
-        <v>#DIV/0!</v>
+        <v>9</v>
       </c>
     </row>
     <row r="12" spans="1:10" ht="16.5" x14ac:dyDescent="0.15">
@@ -4586,13 +4602,15 @@
       <c r="E12" s="9" t="s">
         <v>88</v>
       </c>
-      <c r="F12" s="7"/>
+      <c r="F12" s="7">
+        <v>9</v>
+      </c>
       <c r="G12" s="7"/>
       <c r="H12" s="7"/>
       <c r="I12" s="7"/>
-      <c r="J12" s="6" t="e">
+      <c r="J12" s="6">
         <f>AVERAGE(F12:I12)</f>
-        <v>#DIV/0!</v>
+        <v>9</v>
       </c>
     </row>
     <row r="13" spans="1:10" ht="16.5" x14ac:dyDescent="0.15">
@@ -4611,13 +4629,15 @@
       <c r="E13" s="9" t="s">
         <v>365</v>
       </c>
-      <c r="F13" s="7"/>
+      <c r="F13" s="7">
+        <v>10</v>
+      </c>
       <c r="G13" s="7"/>
       <c r="H13" s="7"/>
       <c r="I13" s="7"/>
-      <c r="J13" s="6" t="e">
+      <c r="J13" s="6">
         <f t="shared" ref="J13:J50" si="0">AVERAGE(F13:I13)</f>
-        <v>#DIV/0!</v>
+        <v>10</v>
       </c>
     </row>
     <row r="14" spans="1:10" ht="16.5" x14ac:dyDescent="0.15">
@@ -4636,13 +4656,15 @@
       <c r="E14" s="9" t="s">
         <v>366</v>
       </c>
-      <c r="F14" s="7"/>
+      <c r="F14" s="7">
+        <v>10</v>
+      </c>
       <c r="G14" s="7"/>
       <c r="H14" s="7"/>
       <c r="I14" s="7"/>
-      <c r="J14" s="6" t="e">
-        <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
+      <c r="J14" s="6">
+        <f t="shared" si="0"/>
+        <v>10</v>
       </c>
     </row>
     <row r="15" spans="1:10" ht="16.5" x14ac:dyDescent="0.15">
@@ -4661,13 +4683,15 @@
       <c r="E15" s="9" t="s">
         <v>241</v>
       </c>
-      <c r="F15" s="7"/>
+      <c r="F15" s="7">
+        <v>8</v>
+      </c>
       <c r="G15" s="7"/>
       <c r="H15" s="7"/>
       <c r="I15" s="7"/>
-      <c r="J15" s="6" t="e">
-        <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
+      <c r="J15" s="6">
+        <f t="shared" si="0"/>
+        <v>8</v>
       </c>
     </row>
     <row r="16" spans="1:10" ht="16.5" x14ac:dyDescent="0.15">
@@ -4686,13 +4710,15 @@
       <c r="E16" s="9" t="s">
         <v>243</v>
       </c>
-      <c r="F16" s="7"/>
+      <c r="F16" s="7">
+        <v>9</v>
+      </c>
       <c r="G16" s="7"/>
       <c r="H16" s="7"/>
       <c r="I16" s="7"/>
-      <c r="J16" s="6" t="e">
-        <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
+      <c r="J16" s="6">
+        <f t="shared" si="0"/>
+        <v>9</v>
       </c>
     </row>
     <row r="17" spans="1:10" ht="16.5" x14ac:dyDescent="0.15">
@@ -4711,13 +4737,15 @@
       <c r="E17" s="9" t="s">
         <v>94</v>
       </c>
-      <c r="F17" s="7"/>
+      <c r="F17" s="7">
+        <v>8</v>
+      </c>
       <c r="G17" s="7"/>
       <c r="H17" s="7"/>
       <c r="I17" s="7"/>
-      <c r="J17" s="6" t="e">
-        <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
+      <c r="J17" s="6">
+        <f t="shared" si="0"/>
+        <v>8</v>
       </c>
     </row>
     <row r="18" spans="1:10" ht="16.5" x14ac:dyDescent="0.15">
@@ -4736,13 +4764,15 @@
       <c r="E18" s="9" t="s">
         <v>95</v>
       </c>
-      <c r="F18" s="7"/>
+      <c r="F18" s="7">
+        <v>9</v>
+      </c>
       <c r="G18" s="7"/>
       <c r="H18" s="7"/>
       <c r="I18" s="7"/>
-      <c r="J18" s="6" t="e">
-        <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
+      <c r="J18" s="6">
+        <f t="shared" si="0"/>
+        <v>9</v>
       </c>
     </row>
     <row r="19" spans="1:10" ht="16.5" x14ac:dyDescent="0.15">
@@ -4761,13 +4791,15 @@
       <c r="E19" s="9" t="s">
         <v>319</v>
       </c>
-      <c r="F19" s="7"/>
+      <c r="F19" s="7">
+        <v>9</v>
+      </c>
       <c r="G19" s="7"/>
       <c r="H19" s="7"/>
       <c r="I19" s="7"/>
-      <c r="J19" s="6" t="e">
-        <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
+      <c r="J19" s="6">
+        <f t="shared" si="0"/>
+        <v>9</v>
       </c>
     </row>
     <row r="20" spans="1:10" ht="16.5" x14ac:dyDescent="0.15">
@@ -4786,13 +4818,15 @@
       <c r="E20" s="9" t="s">
         <v>244</v>
       </c>
-      <c r="F20" s="7"/>
+      <c r="F20" s="7">
+        <v>10</v>
+      </c>
       <c r="G20" s="7"/>
       <c r="H20" s="7"/>
       <c r="I20" s="7"/>
-      <c r="J20" s="6" t="e">
-        <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
+      <c r="J20" s="6">
+        <f t="shared" si="0"/>
+        <v>10</v>
       </c>
     </row>
     <row r="21" spans="1:10" ht="16.5" x14ac:dyDescent="0.15">
@@ -4811,13 +4845,15 @@
       <c r="E21" s="9" t="s">
         <v>172</v>
       </c>
-      <c r="F21" s="7"/>
+      <c r="F21" s="7">
+        <v>9</v>
+      </c>
       <c r="G21" s="7"/>
       <c r="H21" s="7"/>
       <c r="I21" s="7"/>
-      <c r="J21" s="6" t="e">
-        <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
+      <c r="J21" s="6">
+        <f t="shared" si="0"/>
+        <v>9</v>
       </c>
     </row>
     <row r="22" spans="1:10" ht="16.5" x14ac:dyDescent="0.15">
@@ -4836,13 +4872,15 @@
       <c r="E22" s="9" t="s">
         <v>263</v>
       </c>
-      <c r="F22" s="7"/>
+      <c r="F22" s="7">
+        <v>10</v>
+      </c>
       <c r="G22" s="7"/>
       <c r="H22" s="7"/>
       <c r="I22" s="7"/>
-      <c r="J22" s="6" t="e">
-        <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
+      <c r="J22" s="6">
+        <f t="shared" si="0"/>
+        <v>10</v>
       </c>
     </row>
     <row r="23" spans="1:10" ht="16.5" x14ac:dyDescent="0.15">
@@ -4861,13 +4899,15 @@
       <c r="E23" s="9" t="s">
         <v>81</v>
       </c>
-      <c r="F23" s="7"/>
+      <c r="F23" s="7">
+        <v>9</v>
+      </c>
       <c r="G23" s="7"/>
       <c r="H23" s="7"/>
       <c r="I23" s="7"/>
-      <c r="J23" s="6" t="e">
-        <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
+      <c r="J23" s="6">
+        <f t="shared" si="0"/>
+        <v>9</v>
       </c>
     </row>
     <row r="24" spans="1:10" ht="16.5" x14ac:dyDescent="0.15">
@@ -4886,13 +4926,15 @@
       <c r="E24" s="9" t="s">
         <v>173</v>
       </c>
-      <c r="F24" s="7"/>
+      <c r="F24" s="7">
+        <v>10</v>
+      </c>
       <c r="G24" s="7"/>
       <c r="H24" s="7"/>
       <c r="I24" s="7"/>
-      <c r="J24" s="6" t="e">
-        <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
+      <c r="J24" s="6">
+        <f t="shared" si="0"/>
+        <v>10</v>
       </c>
     </row>
     <row r="25" spans="1:10" ht="16.5" x14ac:dyDescent="0.15">
@@ -4911,13 +4953,15 @@
       <c r="E25" s="9" t="s">
         <v>100</v>
       </c>
-      <c r="F25" s="7"/>
+      <c r="F25" s="7">
+        <v>9</v>
+      </c>
       <c r="G25" s="7"/>
       <c r="H25" s="7"/>
       <c r="I25" s="7"/>
-      <c r="J25" s="6" t="e">
-        <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
+      <c r="J25" s="6">
+        <f t="shared" si="0"/>
+        <v>9</v>
       </c>
     </row>
     <row r="26" spans="1:10" ht="16.5" x14ac:dyDescent="0.15">
@@ -4936,13 +4980,15 @@
       <c r="E26" s="9" t="s">
         <v>101</v>
       </c>
-      <c r="F26" s="7"/>
+      <c r="F26" s="7">
+        <v>10</v>
+      </c>
       <c r="G26" s="7"/>
       <c r="H26" s="7"/>
       <c r="I26" s="7"/>
-      <c r="J26" s="6" t="e">
-        <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
+      <c r="J26" s="6">
+        <f t="shared" si="0"/>
+        <v>10</v>
       </c>
     </row>
     <row r="27" spans="1:10" ht="16.5" x14ac:dyDescent="0.15">
@@ -4961,13 +5007,15 @@
       <c r="E27" s="9" t="s">
         <v>30</v>
       </c>
-      <c r="F27" s="7"/>
+      <c r="F27" s="7">
+        <v>10</v>
+      </c>
       <c r="G27" s="7"/>
       <c r="H27" s="7"/>
       <c r="I27" s="7"/>
-      <c r="J27" s="6" t="e">
-        <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
+      <c r="J27" s="6">
+        <f t="shared" si="0"/>
+        <v>10</v>
       </c>
     </row>
     <row r="28" spans="1:10" ht="16.5" x14ac:dyDescent="0.15">
@@ -4986,13 +5034,15 @@
       <c r="E28" s="9" t="s">
         <v>367</v>
       </c>
-      <c r="F28" s="7"/>
+      <c r="F28" s="7">
+        <v>9</v>
+      </c>
       <c r="G28" s="7"/>
       <c r="H28" s="7"/>
       <c r="I28" s="7"/>
-      <c r="J28" s="6" t="e">
-        <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
+      <c r="J28" s="6">
+        <f t="shared" si="0"/>
+        <v>9</v>
       </c>
     </row>
     <row r="29" spans="1:10" ht="16.5" x14ac:dyDescent="0.15">
@@ -5011,13 +5061,15 @@
       <c r="E29" s="9" t="s">
         <v>178</v>
       </c>
-      <c r="F29" s="7"/>
+      <c r="F29" s="7">
+        <v>10</v>
+      </c>
       <c r="G29" s="7"/>
       <c r="H29" s="7"/>
       <c r="I29" s="7"/>
-      <c r="J29" s="6" t="e">
-        <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
+      <c r="J29" s="6">
+        <f t="shared" si="0"/>
+        <v>10</v>
       </c>
     </row>
     <row r="30" spans="1:10" ht="16.5" x14ac:dyDescent="0.15">
@@ -5036,13 +5088,15 @@
       <c r="E30" s="9" t="s">
         <v>325</v>
       </c>
-      <c r="F30" s="7"/>
+      <c r="F30" s="7">
+        <v>8</v>
+      </c>
       <c r="G30" s="7"/>
       <c r="H30" s="7"/>
       <c r="I30" s="7"/>
-      <c r="J30" s="6" t="e">
-        <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
+      <c r="J30" s="6">
+        <f t="shared" si="0"/>
+        <v>8</v>
       </c>
     </row>
     <row r="31" spans="1:10" ht="16.5" x14ac:dyDescent="0.15">
@@ -5061,13 +5115,15 @@
       <c r="E31" s="9" t="s">
         <v>104</v>
       </c>
-      <c r="F31" s="7"/>
+      <c r="F31" s="7">
+        <v>9</v>
+      </c>
       <c r="G31" s="7"/>
       <c r="H31" s="7"/>
       <c r="I31" s="7"/>
-      <c r="J31" s="6" t="e">
-        <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
+      <c r="J31" s="6">
+        <f t="shared" si="0"/>
+        <v>9</v>
       </c>
     </row>
     <row r="32" spans="1:10" ht="16.5" x14ac:dyDescent="0.15">
@@ -5086,13 +5142,15 @@
       <c r="E32" s="9" t="s">
         <v>107</v>
       </c>
-      <c r="F32" s="7"/>
+      <c r="F32" s="7">
+        <v>8</v>
+      </c>
       <c r="G32" s="7"/>
       <c r="H32" s="7"/>
       <c r="I32" s="7"/>
-      <c r="J32" s="6" t="e">
-        <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
+      <c r="J32" s="6">
+        <f t="shared" si="0"/>
+        <v>8</v>
       </c>
     </row>
     <row r="33" spans="1:10" ht="16.5" x14ac:dyDescent="0.15">
@@ -5111,13 +5169,15 @@
       <c r="E33" s="9" t="s">
         <v>329</v>
       </c>
-      <c r="F33" s="7"/>
+      <c r="F33" s="7">
+        <v>9</v>
+      </c>
       <c r="G33" s="7"/>
       <c r="H33" s="7"/>
       <c r="I33" s="7"/>
-      <c r="J33" s="6" t="e">
-        <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
+      <c r="J33" s="6">
+        <f t="shared" si="0"/>
+        <v>9</v>
       </c>
     </row>
     <row r="34" spans="1:10" ht="16.5" x14ac:dyDescent="0.15">
@@ -5136,13 +5196,15 @@
       <c r="E34" s="9" t="s">
         <v>253</v>
       </c>
-      <c r="F34" s="7"/>
+      <c r="F34" s="7">
+        <v>10</v>
+      </c>
       <c r="G34" s="7"/>
       <c r="H34" s="7"/>
       <c r="I34" s="7"/>
-      <c r="J34" s="6" t="e">
-        <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
+      <c r="J34" s="6">
+        <f t="shared" si="0"/>
+        <v>10</v>
       </c>
     </row>
     <row r="35" spans="1:10" ht="16.5" x14ac:dyDescent="0.15">
@@ -5161,13 +5223,15 @@
       <c r="E35" s="9" t="s">
         <v>332</v>
       </c>
-      <c r="F35" s="7"/>
+      <c r="F35" s="7">
+        <v>10</v>
+      </c>
       <c r="G35" s="7"/>
       <c r="H35" s="7"/>
       <c r="I35" s="7"/>
-      <c r="J35" s="6" t="e">
-        <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
+      <c r="J35" s="6">
+        <f t="shared" si="0"/>
+        <v>10</v>
       </c>
     </row>
     <row r="36" spans="1:10" ht="16.5" x14ac:dyDescent="0.15">
@@ -5186,13 +5250,15 @@
       <c r="E36" s="9" t="s">
         <v>16</v>
       </c>
-      <c r="F36" s="7"/>
+      <c r="F36" s="7">
+        <v>9</v>
+      </c>
       <c r="G36" s="7"/>
       <c r="H36" s="7"/>
       <c r="I36" s="7"/>
-      <c r="J36" s="6" t="e">
-        <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
+      <c r="J36" s="6">
+        <f t="shared" si="0"/>
+        <v>9</v>
       </c>
     </row>
     <row r="37" spans="1:10" ht="16.5" x14ac:dyDescent="0.15">
@@ -5211,13 +5277,15 @@
       <c r="E37" s="9" t="s">
         <v>254</v>
       </c>
-      <c r="F37" s="7"/>
+      <c r="F37" s="7">
+        <v>10</v>
+      </c>
       <c r="G37" s="7"/>
       <c r="H37" s="7"/>
       <c r="I37" s="7"/>
-      <c r="J37" s="6" t="e">
-        <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
+      <c r="J37" s="6">
+        <f t="shared" si="0"/>
+        <v>10</v>
       </c>
     </row>
     <row r="38" spans="1:10" ht="16.5" x14ac:dyDescent="0.15">
@@ -5236,13 +5304,15 @@
       <c r="E38" s="9" t="s">
         <v>183</v>
       </c>
-      <c r="F38" s="7"/>
+      <c r="F38" s="7">
+        <v>9</v>
+      </c>
       <c r="G38" s="7"/>
       <c r="H38" s="7"/>
       <c r="I38" s="7"/>
-      <c r="J38" s="6" t="e">
-        <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
+      <c r="J38" s="6">
+        <f t="shared" si="0"/>
+        <v>9</v>
       </c>
     </row>
     <row r="39" spans="1:10" ht="16.5" x14ac:dyDescent="0.15">
@@ -5261,13 +5331,15 @@
       <c r="E39" s="9" t="s">
         <v>257</v>
       </c>
-      <c r="F39" s="7"/>
+      <c r="F39" s="7">
+        <v>10</v>
+      </c>
       <c r="G39" s="7"/>
       <c r="H39" s="7"/>
       <c r="I39" s="7"/>
-      <c r="J39" s="6" t="e">
-        <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
+      <c r="J39" s="6">
+        <f t="shared" si="0"/>
+        <v>10</v>
       </c>
     </row>
     <row r="40" spans="1:10" ht="16.5" x14ac:dyDescent="0.15">
@@ -5286,13 +5358,15 @@
       <c r="E40" s="9" t="s">
         <v>258</v>
       </c>
-      <c r="F40" s="7"/>
+      <c r="F40" s="7">
+        <v>8</v>
+      </c>
       <c r="G40" s="7"/>
       <c r="H40" s="7"/>
       <c r="I40" s="7"/>
-      <c r="J40" s="6" t="e">
-        <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
+      <c r="J40" s="6">
+        <f t="shared" si="0"/>
+        <v>8</v>
       </c>
     </row>
     <row r="41" spans="1:10" ht="16.5" x14ac:dyDescent="0.15">
@@ -5311,13 +5385,15 @@
       <c r="E41" s="9" t="s">
         <v>185</v>
       </c>
-      <c r="F41" s="7"/>
+      <c r="F41" s="7">
+        <v>8</v>
+      </c>
       <c r="G41" s="7"/>
       <c r="H41" s="7"/>
       <c r="I41" s="7"/>
-      <c r="J41" s="6" t="e">
-        <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
+      <c r="J41" s="6">
+        <f t="shared" si="0"/>
+        <v>8</v>
       </c>
     </row>
     <row r="42" spans="1:10" ht="16.5" x14ac:dyDescent="0.15">
@@ -5336,13 +5412,15 @@
       <c r="E42" s="9" t="s">
         <v>109</v>
       </c>
-      <c r="F42" s="7"/>
+      <c r="F42" s="7">
+        <v>9</v>
+      </c>
       <c r="G42" s="7"/>
       <c r="H42" s="7"/>
       <c r="I42" s="7"/>
-      <c r="J42" s="6" t="e">
-        <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
+      <c r="J42" s="6">
+        <f t="shared" si="0"/>
+        <v>9</v>
       </c>
     </row>
     <row r="43" spans="1:10" ht="16.5" x14ac:dyDescent="0.15">
@@ -5361,13 +5439,15 @@
       <c r="E43" s="9" t="s">
         <v>33</v>
       </c>
-      <c r="F43" s="7"/>
+      <c r="F43" s="7">
+        <v>10</v>
+      </c>
       <c r="G43" s="7"/>
       <c r="H43" s="7"/>
       <c r="I43" s="7"/>
-      <c r="J43" s="6" t="e">
-        <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
+      <c r="J43" s="6">
+        <f t="shared" si="0"/>
+        <v>10</v>
       </c>
     </row>
     <row r="44" spans="1:10" ht="16.5" x14ac:dyDescent="0.15">
@@ -5386,13 +5466,15 @@
       <c r="E44" s="9" t="s">
         <v>368</v>
       </c>
-      <c r="F44" s="7"/>
+      <c r="F44" s="7">
+        <v>8</v>
+      </c>
       <c r="G44" s="7"/>
       <c r="H44" s="7"/>
       <c r="I44" s="7"/>
-      <c r="J44" s="6" t="e">
-        <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
+      <c r="J44" s="6">
+        <f t="shared" si="0"/>
+        <v>8</v>
       </c>
     </row>
     <row r="45" spans="1:10" ht="16.5" x14ac:dyDescent="0.15">
@@ -5411,13 +5493,15 @@
       <c r="E45" s="9" t="s">
         <v>189</v>
       </c>
-      <c r="F45" s="7"/>
+      <c r="F45" s="7">
+        <v>10</v>
+      </c>
       <c r="G45" s="7"/>
       <c r="H45" s="7"/>
       <c r="I45" s="7"/>
-      <c r="J45" s="6" t="e">
-        <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
+      <c r="J45" s="6">
+        <f t="shared" si="0"/>
+        <v>10</v>
       </c>
     </row>
     <row r="46" spans="1:10" ht="16.5" x14ac:dyDescent="0.15">
@@ -5436,13 +5520,15 @@
       <c r="E46" s="9" t="s">
         <v>261</v>
       </c>
-      <c r="F46" s="7"/>
+      <c r="F46" s="7">
+        <v>10</v>
+      </c>
       <c r="G46" s="7"/>
       <c r="H46" s="7"/>
       <c r="I46" s="7"/>
-      <c r="J46" s="6" t="e">
-        <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
+      <c r="J46" s="6">
+        <f t="shared" si="0"/>
+        <v>10</v>
       </c>
     </row>
     <row r="47" spans="1:10" ht="16.5" x14ac:dyDescent="0.15">
@@ -5461,13 +5547,15 @@
       <c r="E47" s="9" t="s">
         <v>369</v>
       </c>
-      <c r="F47" s="7"/>
+      <c r="F47" s="7">
+        <v>10</v>
+      </c>
       <c r="G47" s="7"/>
       <c r="H47" s="7"/>
       <c r="I47" s="7"/>
-      <c r="J47" s="6" t="e">
-        <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
+      <c r="J47" s="6">
+        <f t="shared" si="0"/>
+        <v>10</v>
       </c>
     </row>
     <row r="48" spans="1:10" ht="16.5" x14ac:dyDescent="0.15">
@@ -5486,13 +5574,15 @@
       <c r="E48" s="9" t="s">
         <v>101</v>
       </c>
-      <c r="F48" s="7"/>
+      <c r="F48" s="7">
+        <v>10</v>
+      </c>
       <c r="G48" s="7"/>
       <c r="H48" s="7"/>
       <c r="I48" s="7"/>
-      <c r="J48" s="6" t="e">
-        <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
+      <c r="J48" s="6">
+        <f t="shared" si="0"/>
+        <v>10</v>
       </c>
     </row>
     <row r="49" spans="1:10" ht="16.5" x14ac:dyDescent="0.15">
@@ -5511,13 +5601,15 @@
       <c r="E49" s="9" t="s">
         <v>340</v>
       </c>
-      <c r="F49" s="7"/>
+      <c r="F49" s="7">
+        <v>7</v>
+      </c>
       <c r="G49" s="7"/>
       <c r="H49" s="7"/>
       <c r="I49" s="7"/>
-      <c r="J49" s="6" t="e">
-        <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
+      <c r="J49" s="6">
+        <f t="shared" si="0"/>
+        <v>7</v>
       </c>
     </row>
     <row r="50" spans="1:10" ht="16.5" x14ac:dyDescent="0.15">
@@ -5536,13 +5628,15 @@
       <c r="E50" s="9" t="s">
         <v>268</v>
       </c>
-      <c r="F50" s="7"/>
+      <c r="F50" s="7">
+        <v>10</v>
+      </c>
       <c r="G50" s="7"/>
       <c r="H50" s="7"/>
       <c r="I50" s="7"/>
-      <c r="J50" s="6" t="e">
-        <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
+      <c r="J50" s="6">
+        <f t="shared" si="0"/>
+        <v>10</v>
       </c>
     </row>
     <row r="51" spans="1:10" ht="16.5" x14ac:dyDescent="0.15">
@@ -5561,13 +5655,15 @@
       <c r="E51" s="9" t="s">
         <v>113</v>
       </c>
-      <c r="F51" s="7"/>
+      <c r="F51" s="7">
+        <v>8</v>
+      </c>
       <c r="G51" s="7"/>
       <c r="H51" s="7"/>
       <c r="I51" s="7"/>
-      <c r="J51" s="6" t="e">
+      <c r="J51" s="6">
         <f t="shared" ref="J51" si="1">AVERAGE(F51:I51)</f>
-        <v>#DIV/0!</v>
+        <v>8</v>
       </c>
     </row>
   </sheetData>
@@ -5600,8 +5696,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C71A6A0A-D35A-46D3-AE05-F9914FF9FBE0}">
   <dimension ref="A1:J51"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B34" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="F34" sqref="F34"/>
+    <sheetView topLeftCell="B1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="F3" sqref="F3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -5672,7 +5768,7 @@
       <c r="D3" s="14"/>
       <c r="E3" s="17"/>
       <c r="F3" s="3">
-        <v>44826</v>
+        <v>44096</v>
       </c>
       <c r="G3" s="3" t="s">
         <v>12</v>

</xml_diff>